<commit_message>
Add vpa_data_description.md for detailed documentation on VPA Data Module and its classes
</commit_message>
<xml_diff>
--- a/cross_correlation_functions.xlsx
+++ b/cross_correlation_functions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aspire5 15 i7 4G2050\vpa_modular_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{325C79D2-DE18-4BE2-9778-918D5D8156DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E84ADF-7F65-416B-A91D-87829705FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D33C2490-AD92-42FE-8AEA-2B2C19B12E50}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D33C2490-AD92-42FE-8AEA-2B2C19B12E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,6 +36,73 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="4">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+  <valueMetadata count="4">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+    <bk>
+      <rc t="2" v="2"/>
+    </bk>
+    <bk>
+      <rc t="2" v="3"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="115">
   <si>
@@ -387,6 +455,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -567,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -579,12 +650,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -602,57 +667,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1032,13 +1060,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1051,6 +1072,59 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1066,21 +1140,848 @@
 </styleSheet>
 </file>
 
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+  <types>
+    <type name="_imageurl">
+      <keyFlags>
+        <key name="Blip Identifier">
+          <flag name="ShowInCardView" value="0"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentity">
+      <keyFlags>
+        <key name="%cvi">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+    <type name="_linkedentitycore">
+      <keyFlags>
+        <key name="%EntityServiceId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntitySubDomainId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityCulture">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%EntityId">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%IsRefreshable">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+        <key name="%ProviderInfo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLinkLogo">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%DataProviderExternalLink">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+        </key>
+        <key name="%OutdatedReason">
+          <flag name="ShowInCardView" value="0"/>
+          <flag name="ShowInDotNotation" value="0"/>
+          <flag name="ShowInAutoComplete" value="0"/>
+          <flag name="ExcludeFromCalcComparison" value="1"/>
+        </key>
+      </keyFlags>
+    </type>
+  </types>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="16">
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1ygoc&amp;q=XNAS%3aNFLX&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-AE</v>
+    <v>a1ygoc</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>NETFLIX, INC. (XNAS:NFLX)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>1159.44</v>
+    <v>555.59</v>
+    <v>1.6066</v>
+    <v>23.02</v>
+    <v>-9.683999999999999E-4</v>
+    <v>2.0309000000000001E-2</v>
+    <v>-1.1200000000000001</v>
+    <v>USD</v>
+    <v>Netflix, Inc. is a provider of entertainment services. The Company acquires, licenses and produces content, including original programming. It provides paid memberships in over 190 countries offering television (TV) series, films and games across a variety of genres and languages. It allows members to play, pause and resume watching as much as they want, anytime, anywhere, and can change their plans at any time. The Company offers members the ability to receive streaming content through a host of Internet-connected devices, including TVs, digital video players, TV set-top boxes and mobile devices. It is engaged in scaling its streaming service, such as introducing games and advertising on its service, as well as offering live programming. It is developing technology and utilizing third-party cloud computing, technology and other services. The Company is also engaged in scaling its own studio operations to produce original content.</v>
+    <v>14000</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>121 Albright Way, LOS GATOS, CA, 95032 US</v>
+    <v>1159.44</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>45779.95308165469</v>
+    <v>0</v>
+    <v>1133.32</v>
+    <v>492168952737</v>
+    <v>NETFLIX, INC.</v>
+    <v>NETFLIX, INC.</v>
+    <v>1136.6600000000001</v>
+    <v>54.645200000000003</v>
+    <v>1133.47</v>
+    <v>1156.49</v>
+    <v>1155.3699999999999</v>
+    <v>425571300</v>
+    <v>NFLX</v>
+    <v>NETFLIX, INC. (XNAS:NFLX)</v>
+    <v>3769325</v>
+    <v>5542343</v>
+    <v>1997</v>
+  </rv>
+  <rv s="2">
+    <v>1</v>
+  </rv>
+  <rv s="0">
+    <v>http://en.wikipedia.org/wiki/Public_domain</v>
+    <v>Public domain</v>
+  </rv>
+  <rv s="0">
+    <v>https://en.wikipedia.org/wiki/Microsoft</v>
+    <v>Wikipedia</v>
+  </rv>
+  <rv s="3">
+    <v>3</v>
+    <v>4</v>
+  </rv>
+  <rv s="4">
+    <v>9</v>
+    <v>https://www.bing.com/th?id=AMMS_e6e837c7bf3a77408619758b7447855a&amp;qlt=95</v>
+    <v>5</v>
+    <v>0</v>
+    <v>https://www.bing.com/images/search?form=xlimg&amp;q=microsoft</v>
+    <v>Image of MICROSOFT CORPORATION</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1xzim&amp;q=XNAS%3aMSFT&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="5">
+    <v>en-AE</v>
+    <v>a1xzim</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>5</v>
+    <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
+    <v>7</v>
+    <v>8</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>468.35</v>
+    <v>344.79</v>
+    <v>0.98909999999999998</v>
+    <v>9.8800000000000008</v>
+    <v>-5.2839999999999994E-4</v>
+    <v>2.3224999999999999E-2</v>
+    <v>-0.23</v>
+    <v>USD</v>
+    <v>Microsoft Corporation is a technology company. The Company develops and supports software, services, devices, and solutions. The Company’s segments include Productivity and Business Processes, Intelligent Cloud, and More Personal Computing. The Productivity and Business Processes segment consists of products and services in its portfolio of productivity, communication, and information services. This segment primarily comprises: Office Commercial, Office Consumer, LinkedIn, and Dynamics business solutions. The Intelligent Cloud segment consists of server products and cloud services, including Azure and other cloud services, SQL Server, Windows Server, Visual Studio, System Center, and related Client Access Licenses (CALs), and Nuance and GitHub; and Enterprise Services, including enterprise support services, industry solutions and Nuance professional services. The More Personal Computing segment primarily comprises Windows, Devices, Gaming, and search and news advertising.</v>
+    <v>228000</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>One Microsoft Way, REDMOND, WA, 98052 US</v>
+    <v>439.44</v>
+    <v>6</v>
+    <v>Software &amp; IT Services</v>
+    <v>Stock</v>
+    <v>45779.95330887656</v>
+    <v>7</v>
+    <v>429.98500000000001</v>
+    <v>3235237752320</v>
+    <v>MICROSOFT CORPORATION</v>
+    <v>MICROSOFT CORPORATION</v>
+    <v>431.74</v>
+    <v>33.639600000000002</v>
+    <v>425.4</v>
+    <v>435.28</v>
+    <v>435.05</v>
+    <v>7432544000</v>
+    <v>MSFT</v>
+    <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
+    <v>30747812</v>
+    <v>27706619</v>
+    <v>1993</v>
+  </rv>
+  <rv s="2">
+    <v>8</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1nhlh&amp;q=XNAS%3aAMZN&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-AE</v>
+    <v>a1nhlh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>242.52</v>
+    <v>151.61000000000001</v>
+    <v>1.3252999999999999</v>
+    <v>-0.22</v>
+    <v>-1.5789999999999999E-4</v>
+    <v>-1.157E-3</v>
+    <v>-0.03</v>
+    <v>USD</v>
+    <v>Amazon.com, Inc. provides a range of products and services to customers. The products offered through its stores include merchandise and content it has purchased for resale and products offered by third-party sellers. The Company’s segments include North America, International and Amazon Web Services (AWS). It serves consumers through its online and physical stores and focuses on selection, price, and convenience. Customers access its offerings through its websites, mobile apps, Alexa, devices, streaming, and physically visiting its stores. It also manufactures and sells electronic devices, including Kindle, Fire tablet, Fire TV, Echo, Ring, Blink, and eero, and develops and produces media content. It serves developers and enterprises of all sizes, including start-ups, government agencies, and academic institutions, through AWS, which offers a set of on-demand technology services, including compute, storage, database, analytics, and machine learning, and other services.</v>
+    <v>1556000</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>410 Terry Avenue North, SEATTLE, WA, 98109 US</v>
+    <v>192.88</v>
+    <v>Diversified Retail</v>
+    <v>Stock</v>
+    <v>45779.953310057812</v>
+    <v>10</v>
+    <v>186.4</v>
+    <v>2018472000000</v>
+    <v>AMAZON.COM, INC.</v>
+    <v>AMAZON.COM, INC.</v>
+    <v>191.435</v>
+    <v>31.019600000000001</v>
+    <v>190.2</v>
+    <v>189.98</v>
+    <v>189.95</v>
+    <v>10612360000</v>
+    <v>AMZN</v>
+    <v>AMAZON.COM, INC. (XNAS:AMZN)</v>
+    <v>77843282</v>
+    <v>61230915</v>
+    <v>1996</v>
+  </rv>
+  <rv s="2">
+    <v>11</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a24kar&amp;q=XNAS%3aTSLA&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>en-AE</v>
+    <v>a24kar</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>0</v>
+    <v>TESLA, INC. (XNAS:TSLA)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>488.53989999999999</v>
+    <v>167.41</v>
+    <v>2.4510000000000001</v>
+    <v>6.69</v>
+    <v>1.7060000000000001E-3</v>
+    <v>2.3848999999999999E-2</v>
+    <v>0.49</v>
+    <v>USD</v>
+    <v>Tesla, Inc. designs, develops, manufactures, sells and leases high-performance fully electric vehicles and energy generation and storage systems, and offers services related to its products. Its segments include automotive, and energy generation and storage. The automotive segment includes the design, development, manufacturing, sales and leasing of high-performance fully electric vehicles, and sales of automotive regulatory credits. It also includes sales of used vehicles, non-warranty maintenance services and collisions, part sales, paid supercharging, insurance services revenue and retail merchandise sales. The energy generation and storage segment include the design, manufacture, installation, sales and leasing of solar energy generation and energy storage products and related services and sales of solar energy systems incentives. Its consumer vehicles include the Model 3, Y, S, X and Cybertruck. Its lithium-ion battery energy storage products include Powerwall and Megapack.</v>
+    <v>125665</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>1 Tesla Road, AUSTIN, TX, 78725 US</v>
+    <v>294.77999999999997</v>
+    <v>Automobiles &amp; Auto Parts</v>
+    <v>Stock</v>
+    <v>45779.953204733596</v>
+    <v>13</v>
+    <v>279.81</v>
+    <v>925090772759</v>
+    <v>TESLA, INC.</v>
+    <v>TESLA, INC.</v>
+    <v>284.89999999999998</v>
+    <v>154.3974</v>
+    <v>280.52</v>
+    <v>287.20999999999998</v>
+    <v>287.7</v>
+    <v>3220956000</v>
+    <v>TSLA</v>
+    <v>TESLA, INC. (XNAS:TSLA)</v>
+    <v>114214271</v>
+    <v>139121393</v>
+    <v>2024</v>
+  </rv>
+  <rv s="2">
+    <v>14</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
+  <s t="_hyperlink">
+    <k n="Address" t="s"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change % (Extended hours)"/>
+    <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Price (Extended hours)"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentity">
+    <k n="%cvi" t="r"/>
+  </s>
+  <s t="_sourceattribution">
+    <k n="License" t="r"/>
+    <k n="Source" t="r"/>
+  </s>
+  <s t="_imageurl">
+    <k n="_Provider" t="spb"/>
+    <k n="Address" t="s"/>
+    <k n="Attribution" t="r"/>
+    <k n="ComputedImage" t="b"/>
+    <k n="More Images Address" t="s"/>
+    <k n="Text" t="s"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change % (Extended hours)"/>
+    <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Image" t="r"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Price (Extended hours)"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
+<supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+  <spbArrays count="2">
+    <a count="45">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+    <a count="46">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">Image</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+  </spbArrays>
+  <spbData count="10">
+    <spb s="0">
+      <v>0</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="1">
+      <v>0</v>
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="2">
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+    </spb>
+    <spb s="3">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
+    </spb>
+    <spb s="4">
+      <v>at close</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from close</v>
+      <v>from close</v>
+    </spb>
+    <spb s="0">
+      <v>1</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="5">
+      <v>0</v>
+      <v>0</v>
+    </spb>
+    <spb s="6">
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+    </spb>
+    <spb s="7">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>10</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
+    </spb>
+    <spb s="8">
+      <v>Powered by Refinitiv</v>
+    </spb>
+  </spbData>
+</supportingPropertyBags>
+</file>
+
+<file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
+  <s>
+    <k n="^Order" t="spba"/>
+    <k n="TitleProperty" t="s"/>
+    <k n="SubTitleProperty" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInCardView" t="b"/>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="ExchangeID" t="spb"/>
+    <k n="UniqueName" t="spb"/>
+    <k n="`%ProviderInfo" t="spb"/>
+    <k n="LearnMoreOnLink" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
+  </s>
+  <s>
+    <k n="ShowInDotNotation" t="b"/>
+    <k n="ShowInAutoComplete" t="b"/>
+  </s>
+  <s>
+    <k n="Image" t="spb"/>
+    <k n="ExchangeID" t="spb"/>
+    <k n="UniqueName" t="spb"/>
+    <k n="`%ProviderInfo" t="spb"/>
+    <k n="LearnMoreOnLink" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Image" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="name" t="s"/>
+  </s>
+</spbStructures>
+</file>
+
+<file path=xl/richData/richStyles.xml><?xml version="1.0" encoding="utf-8"?>
+<richStyleSheet xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <dxfs count="7">
+    <x:dxf>
+      <x:numFmt numFmtId="2" formatCode="0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="0" formatCode="General"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="14" formatCode="0.00%"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="3" formatCode="#,##0"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="4" formatCode="#,##0.00"/>
+    </x:dxf>
+    <x:dxf>
+      <x:numFmt numFmtId="1" formatCode="0"/>
+    </x:dxf>
+  </dxfs>
+  <richProperties>
+    <rPr n="NumberFormat" t="s"/>
+    <rPr n="IsTitleField" t="b"/>
+    <rPr n="IsHeroField" t="b"/>
+  </richProperties>
+  <richStyles>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0.00_);_([$$-en-US]* (#,##0.00);_([$$-en-US]* "-"??_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="5">
+      <rpv i="0">#,##0.00</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="1">1</rpv>
+    </rSty>
+    <rSty dxfid="4">
+      <rpv i="0">#,##0</rpv>
+    </rSty>
+    <rSty dxfid="3"/>
+    <rSty dxfid="1">
+      <rpv i="0">_([$$-en-US]* #,##0_);_([$$-en-US]* (#,##0);_([$$-en-US]* "-"_);_(@_)</rpv>
+    </rSty>
+    <rSty dxfid="2"/>
+    <rSty dxfid="6">
+      <rpv i="0">0</rpv>
+    </rSty>
+    <rSty dxfid="0">
+      <rpv i="0">0.00</rpv>
+    </rSty>
+    <rSty>
+      <rpv i="2">1</rpv>
+    </rSty>
+  </richStyles>
+</richStyleSheet>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4885A52A-1AFD-48E5-901C-8A39290CB697}" name="Table1" displayName="Table1" ref="F2:P120" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4885A52A-1AFD-48E5-901C-8A39290CB697}" name="Table1" displayName="Table1" ref="F2:P120" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="F2:P120" xr:uid="{4885A52A-1AFD-48E5-901C-8A39290CB697}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{CB50A1F3-E816-4011-8569-C92FBF7F4E45}" name="vpa_config.py" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{42A06F41-77CC-414E-81FF-452EBCC67D40}" name="vpa_analyzer.py" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{CA8BF3C7-0A74-403B-82CE-72DE0365B164}" name="vpa_data.py" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{9BF9B2C9-BAE4-484F-BC05-CC9162A7B092}" name="vpa_facade.py" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{6012B60C-3F54-4ABB-B5B6-6EB493448A47}" name="vpa_llm_interface.py" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{36CCA757-582A-48AF-A3A1-8A83D12D45C3}" name="vpa_logger.py" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{665D1EBB-FAD9-4DAB-8836-C54C7DDADDDD}" name="vp_processor.py" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{A4905A25-154A-4E4E-B664-21B484723BC8}" name="vpa_signals.py" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{1F8E4A00-E8A5-4276-8B6A-8B35426156D8}" name="vpa_utills.py" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{D85C25DA-9717-47CE-A12C-3F5B33DDC6C2}" name="vpa_llm_query_engine" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{BB2AB252-61D5-4D26-97EF-B7AF8E897319}" name="vpa_training_data_generator" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CB50A1F3-E816-4011-8569-C92FBF7F4E45}" name="vpa_config.py" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{42A06F41-77CC-414E-81FF-452EBCC67D40}" name="vpa_analyzer.py" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CA8BF3C7-0A74-403B-82CE-72DE0365B164}" name="vpa_data.py" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{9BF9B2C9-BAE4-484F-BC05-CC9162A7B092}" name="vpa_facade.py" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{6012B60C-3F54-4ABB-B5B6-6EB493448A47}" name="vpa_llm_interface.py" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{36CCA757-582A-48AF-A3A1-8A83D12D45C3}" name="vpa_logger.py" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{665D1EBB-FAD9-4DAB-8836-C54C7DDADDDD}" name="vp_processor.py" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{A4905A25-154A-4E4E-B664-21B484723BC8}" name="vpa_signals.py" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1F8E4A00-E8A5-4276-8B6A-8B35426156D8}" name="vpa_utills.py" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{D85C25DA-9717-47CE-A12C-3F5B33DDC6C2}" name="vpa_llm_query_engine" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{BB2AB252-61D5-4D26-97EF-B7AF8E897319}" name="vpa_training_data_generator" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1401,12 +2302,98 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="619" row="4">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="597" row="5">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1B24233E-BEEE-475C-88EC-6E4F3C6236B1}">
+  <we:reference id="wa104379220" version="8.0.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA104379220" version="8.0.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="Office.AutoShowTaskpaneWithDocument" value="true"/>
+    <we:property name="stocksChange" value="{}"/>
+    <we:property name="stocks" value="{}"/>
+    <we:property name="stocksOrder" value="[]"/>
+    <we:property name="updateIntervalIndex" value="2"/>
+    <we:property name="stocksSources" value="{}"/>
+    <we:property name="lastCryptoCompare" value="0"/>
+    <we:property name="lastIexCall" value="0"/>
+    <we:property name="lastMutualFundsCall" value="0"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{BC746A0C-6342-43D7-BE3A-C768E6CF8EF3}">
+  <we:reference id="wa200003886" version="1.0.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200003886" version="1.0.0.0" store="WA200003886" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_FS_TEST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_REVENUEBREAKDOWN</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_HISTORICALMARKETCAP</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_DIVIDENDS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_INSTITUTIONALPORTFOLIOS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EARNINGSCALENDAR</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EQUITYTICK</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_SHORTINTEREST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_OPTIONEXPIRATIONDATES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_OPTIONCHAIN</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EQUITYMETRICS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EQUITYFULLFINANCIALS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EQUITYCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_FOREXCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_CRYPTOCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_ETFCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_MUTUALFUNDCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_FOREXALLRATES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_CRYPTOPROFILE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_ETFPROFILE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_MUTUALFUNDPROFILE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_LATEST</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_STREAMING</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_PATTERNRECOGNITION</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_SUPPORTRESISTANCE</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_AGGREGATEINDICATORS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_TECHNICALINDICATORS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_ESG</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_EARNINGSQUALITY</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_API</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_ETFHOLDINGS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_MUTUALFUNDHOLDINGS</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_BONDCANDLES</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_BONDTICK</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_FS_FUTURESCANDLES</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8A70AD-6748-4773-971A-D413622CBF2C}">
   <dimension ref="D2:P120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M107" sqref="M107"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,44 +2409,44 @@
     <col min="12" max="12" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.77734375" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1468,7 +2455,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1478,239 +2465,239 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="11"/>
+      <c r="P3" s="9"/>
     </row>
     <row r="4" spans="4:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M4" s="18" t="s">
+      <c r="L4" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="11"/>
+      <c r="P4" s="9"/>
     </row>
     <row r="5" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="18" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M5" s="18" t="s">
+      <c r="L5" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="11"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="18" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M6" s="18" t="s">
+      <c r="L6" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="11"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="18" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M7" s="18" t="s">
+      <c r="L7" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M7" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="11"/>
+      <c r="P7" s="9"/>
     </row>
     <row r="8" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="18" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M8" s="18" t="s">
+      <c r="L8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M8" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="11"/>
+      <c r="P8" s="9"/>
     </row>
     <row r="9" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="18" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M9" s="18" t="s">
+      <c r="L9" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="11"/>
+      <c r="P9" s="9"/>
     </row>
     <row r="10" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="18" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M10" s="18" t="s">
+      <c r="L10" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="11"/>
+      <c r="P10" s="9"/>
     </row>
     <row r="11" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="18" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H11" s="4"/>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="11"/>
+      <c r="P11" s="9"/>
     </row>
     <row r="12" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="18" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="16" t="s">
         <v>114</v>
       </c>
       <c r="H12" s="4"/>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="16" t="s">
         <v>114</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="M12" s="18" t="s">
+      <c r="L12" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="M12" s="16" t="s">
         <v>114</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="11"/>
+      <c r="P12" s="9"/>
     </row>
     <row r="13" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1720,14 +2707,14 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="11"/>
+      <c r="P13" s="9"/>
     </row>
     <row r="14" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="10"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1737,14 +2724,14 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="11"/>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1754,14 +2741,14 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="11"/>
+      <c r="P15" s="9"/>
     </row>
     <row r="16" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1771,14 +2758,14 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="11"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="10"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1788,14 +2775,14 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="11"/>
+      <c r="P17" s="9"/>
     </row>
     <row r="18" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="10"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1805,14 +2792,14 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="11"/>
+      <c r="P18" s="9"/>
     </row>
     <row r="19" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="10"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1822,14 +2809,14 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="11"/>
+      <c r="P19" s="9"/>
     </row>
     <row r="20" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="10"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1839,14 +2826,14 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="11"/>
+      <c r="P20" s="9"/>
     </row>
     <row r="21" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1856,14 +2843,14 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="11"/>
+      <c r="P21" s="9"/>
     </row>
     <row r="22" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="10"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1873,14 +2860,14 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="11"/>
+      <c r="P22" s="9"/>
     </row>
     <row r="23" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="10"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -1890,14 +2877,14 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="11"/>
+      <c r="P23" s="9"/>
     </row>
     <row r="24" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="10"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1907,14 +2894,14 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="11"/>
+      <c r="P24" s="9"/>
     </row>
     <row r="25" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="10"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1924,14 +2911,14 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="11"/>
+      <c r="P25" s="9"/>
     </row>
     <row r="26" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="10"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1941,14 +2928,14 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="11"/>
+      <c r="P26" s="9"/>
     </row>
     <row r="27" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="10"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="8"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1958,14 +2945,14 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="11"/>
+      <c r="P27" s="9"/>
     </row>
     <row r="28" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="10"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1975,14 +2962,14 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="11"/>
+      <c r="P28" s="9"/>
     </row>
     <row r="29" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="10"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="8"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -1992,17 +2979,17 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="11"/>
+      <c r="P29" s="9"/>
     </row>
     <row r="30" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="10"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J30" s="4"/>
@@ -2011,17 +2998,17 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="11"/>
+      <c r="P30" s="9"/>
     </row>
     <row r="31" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="10"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="8"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="19" t="s">
+      <c r="I31" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J31" s="4"/>
@@ -2030,17 +3017,17 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="11"/>
+      <c r="P31" s="9"/>
     </row>
     <row r="32" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="10"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="8"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J32" s="4"/>
@@ -2049,14 +3036,14 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="11"/>
+      <c r="P32" s="9"/>
     </row>
     <row r="33" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="10"/>
+      <c r="F33" s="8"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
@@ -2066,14 +3053,14 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="11"/>
+      <c r="P33" s="9"/>
     </row>
     <row r="34" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D34" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="10"/>
+      <c r="F34" s="8"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
@@ -2083,14 +3070,14 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="11"/>
+      <c r="P34" s="9"/>
     </row>
     <row r="35" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="10"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="8"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
@@ -2100,14 +3087,14 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="11"/>
+      <c r="P35" s="9"/>
     </row>
     <row r="36" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="10"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="8"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -2117,14 +3104,14 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="11"/>
+      <c r="P36" s="9"/>
     </row>
     <row r="37" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="10"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="8"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -2134,17 +3121,17 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
-      <c r="P37" s="11"/>
+      <c r="P37" s="9"/>
     </row>
     <row r="38" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D38" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="10"/>
+      <c r="F38" s="8"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="19" t="s">
+      <c r="I38" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J38" s="4"/>
@@ -2153,19 +3140,19 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
-      <c r="P38" s="19" t="s">
+      <c r="P38" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="39" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="10"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="19" t="s">
+      <c r="I39" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J39" s="4"/>
@@ -2174,19 +3161,19 @@
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
-      <c r="P39" s="19" t="s">
+      <c r="P39" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="40" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="10"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="8"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="19" t="s">
+      <c r="I40" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J40" s="4"/>
@@ -2195,19 +3182,19 @@
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
-      <c r="P40" s="19" t="s">
+      <c r="P40" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="10"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="8"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="19" t="s">
+      <c r="I41" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J41" s="4"/>
@@ -2216,7 +3203,7 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
-      <c r="P41" s="19" t="s">
+      <c r="P41" s="17" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2225,7 +3212,7 @@
         <v>36</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="10"/>
+      <c r="F42" s="8"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -2235,14 +3222,14 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
-      <c r="P42" s="11"/>
+      <c r="P42" s="9"/>
     </row>
     <row r="43" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="10"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="8"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
@@ -2252,14 +3239,14 @@
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
-      <c r="P43" s="11"/>
+      <c r="P43" s="9"/>
     </row>
     <row r="44" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="10"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="8"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
@@ -2269,14 +3256,14 @@
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
-      <c r="P44" s="11"/>
+      <c r="P44" s="9"/>
     </row>
     <row r="45" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="10"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="8"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
@@ -2286,17 +3273,17 @@
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
-      <c r="P45" s="11"/>
+      <c r="P45" s="9"/>
     </row>
     <row r="46" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D46" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="10"/>
+      <c r="F46" s="8"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="19" t="s">
+      <c r="I46" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J46" s="4"/>
@@ -2305,17 +3292,17 @@
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
-      <c r="P46" s="11"/>
+      <c r="P46" s="9"/>
     </row>
     <row r="47" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="10"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="8"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
-      <c r="I47" s="19" t="s">
+      <c r="I47" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J47" s="4"/>
@@ -2324,14 +3311,14 @@
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
-      <c r="P47" s="11"/>
+      <c r="P47" s="9"/>
     </row>
     <row r="48" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="6" t="s">
         <v>39</v>
       </c>
       <c r="E48" s="4"/>
-      <c r="F48" s="10"/>
+      <c r="F48" s="8"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -2341,175 +3328,175 @@
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
-      <c r="P48" s="11"/>
+      <c r="P48" s="9"/>
     </row>
     <row r="49" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D49" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E49" s="4"/>
-      <c r="F49" s="10"/>
+      <c r="F49" s="8"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="19" t="s">
+      <c r="J49" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P49" s="19" t="s">
+      <c r="O49" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P49" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="50" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="10"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="8"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="19" t="s">
+      <c r="J50" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P50" s="19" t="s">
+      <c r="O50" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P50" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="51" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E51" s="7"/>
-      <c r="F51" s="10"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="8"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="19" t="s">
+      <c r="J51" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P51" s="19" t="s">
+      <c r="O51" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P51" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="52" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="10"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="8"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="19" t="s">
+      <c r="J52" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P52" s="19" t="s">
+      <c r="O52" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P52" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="53" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E53" s="7"/>
-      <c r="F53" s="10"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="8"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="19" t="s">
+      <c r="J53" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P53" s="19" t="s">
+      <c r="O53" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P53" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="54" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="7"/>
-      <c r="F54" s="10"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="8"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="19" t="s">
+      <c r="J54" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P54" s="19" t="s">
+      <c r="O54" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P54" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="55" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D55" s="6" t="s">
+      <c r="D55" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="10"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="8"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="19" t="s">
+      <c r="J55" s="17" t="s">
         <v>114</v>
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="P55" s="19" t="s">
+      <c r="O55" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="P55" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D56" s="8" t="s">
+      <c r="D56" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="F56" s="10"/>
+      <c r="F56" s="8"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -2519,14 +3506,14 @@
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
-      <c r="P56" s="11"/>
+      <c r="P56" s="9"/>
     </row>
     <row r="57" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D57" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="F57" s="10"/>
+      <c r="F57" s="8"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -2536,14 +3523,14 @@
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
-      <c r="P57" s="11"/>
+      <c r="P57" s="9"/>
     </row>
     <row r="58" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E58" s="7"/>
-      <c r="F58" s="10"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="8"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -2553,14 +3540,14 @@
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
-      <c r="P58" s="11"/>
+      <c r="P58" s="9"/>
     </row>
     <row r="59" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E59" s="7"/>
-      <c r="F59" s="10"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="8"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -2570,14 +3557,14 @@
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
-      <c r="P59" s="11"/>
+      <c r="P59" s="9"/>
     </row>
     <row r="60" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E60" s="7"/>
-      <c r="F60" s="10"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="8"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -2587,14 +3574,14 @@
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
-      <c r="P60" s="11"/>
+      <c r="P60" s="9"/>
     </row>
     <row r="61" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="7"/>
-      <c r="F61" s="10"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="8"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -2604,14 +3591,14 @@
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
-      <c r="P61" s="11"/>
+      <c r="P61" s="9"/>
     </row>
     <row r="62" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E62" s="7"/>
-      <c r="F62" s="10"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="8"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -2621,14 +3608,14 @@
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
-      <c r="P62" s="11"/>
+      <c r="P62" s="9"/>
     </row>
     <row r="63" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E63" s="7"/>
-      <c r="F63" s="10"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="8"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -2638,14 +3625,14 @@
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
-      <c r="P63" s="11"/>
+      <c r="P63" s="9"/>
     </row>
     <row r="64" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="6" t="s">
         <v>55</v>
       </c>
       <c r="E64" s="4"/>
-      <c r="F64" s="10"/>
+      <c r="F64" s="8"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -2655,17 +3642,17 @@
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
       <c r="O64" s="4"/>
-      <c r="P64" s="11"/>
+      <c r="P64" s="9"/>
     </row>
     <row r="65" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D65" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E65" s="4"/>
-      <c r="F65" s="10"/>
+      <c r="F65" s="8"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="19" t="s">
+      <c r="I65" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J65" s="4"/>
@@ -2674,19 +3661,19 @@
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
-      <c r="P65" s="19" t="s">
+      <c r="P65" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="66" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="E66" s="7"/>
-      <c r="F66" s="10"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="8"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="19" t="s">
+      <c r="I66" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J66" s="4"/>
@@ -2695,19 +3682,19 @@
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
       <c r="O66" s="4"/>
-      <c r="P66" s="19" t="s">
+      <c r="P66" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="67" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E67" s="7"/>
-      <c r="F67" s="10"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="8"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="19" t="s">
+      <c r="I67" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J67" s="4"/>
@@ -2716,19 +3703,19 @@
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
       <c r="O67" s="4"/>
-      <c r="P67" s="19" t="s">
+      <c r="P67" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="68" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E68" s="7"/>
-      <c r="F68" s="10"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="8"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
-      <c r="I68" s="19" t="s">
+      <c r="I68" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J68" s="4"/>
@@ -2737,19 +3724,19 @@
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
-      <c r="P68" s="19" t="s">
+      <c r="P68" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="69" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E69" s="7"/>
-      <c r="F69" s="10"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="8"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="19" t="s">
+      <c r="I69" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J69" s="4"/>
@@ -2758,19 +3745,19 @@
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
-      <c r="P69" s="19" t="s">
+      <c r="P69" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="70" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="10"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="8"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="19" t="s">
+      <c r="I70" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J70" s="4"/>
@@ -2779,19 +3766,19 @@
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
-      <c r="P70" s="19" t="s">
+      <c r="P70" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="71" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E71" s="7"/>
-      <c r="F71" s="10"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="8"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="19" t="s">
+      <c r="I71" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J71" s="4"/>
@@ -2800,19 +3787,19 @@
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
-      <c r="P71" s="19" t="s">
+      <c r="P71" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="72" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D72" s="6" t="s">
+      <c r="D72" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E72" s="7"/>
-      <c r="F72" s="10"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="8"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
-      <c r="I72" s="19" t="s">
+      <c r="I72" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J72" s="4"/>
@@ -2821,19 +3808,19 @@
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
-      <c r="P72" s="19" t="s">
+      <c r="P72" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="73" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="F73" s="10"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="8"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
-      <c r="I73" s="19" t="s">
+      <c r="I73" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J73" s="4"/>
@@ -2842,19 +3829,19 @@
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
-      <c r="P73" s="19" t="s">
+      <c r="P73" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="74" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E74" s="7"/>
-      <c r="F74" s="10"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="8"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
-      <c r="I74" s="19" t="s">
+      <c r="I74" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J74" s="4"/>
@@ -2863,19 +3850,19 @@
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
       <c r="O74" s="4"/>
-      <c r="P74" s="19" t="s">
+      <c r="P74" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="75" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D75" s="6" t="s">
+      <c r="D75" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E75" s="7"/>
-      <c r="F75" s="10"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="8"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
-      <c r="I75" s="19" t="s">
+      <c r="I75" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J75" s="4"/>
@@ -2884,19 +3871,19 @@
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
-      <c r="P75" s="19" t="s">
+      <c r="P75" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="76" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D76" s="6" t="s">
+      <c r="D76" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E76" s="7"/>
-      <c r="F76" s="10"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="8"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
-      <c r="I76" s="19" t="s">
+      <c r="I76" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J76" s="4"/>
@@ -2905,19 +3892,19 @@
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
       <c r="O76" s="4"/>
-      <c r="P76" s="19" t="s">
+      <c r="P76" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="77" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D77" s="6" t="s">
+      <c r="D77" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E77" s="7"/>
-      <c r="F77" s="10"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="8"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
-      <c r="I77" s="19" t="s">
+      <c r="I77" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J77" s="4"/>
@@ -2926,16 +3913,16 @@
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
       <c r="O77" s="4"/>
-      <c r="P77" s="19" t="s">
+      <c r="P77" s="17" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="78" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D78" s="8" t="s">
+      <c r="D78" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E78" s="4"/>
-      <c r="F78" s="10"/>
+      <c r="F78" s="8"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
@@ -2945,182 +3932,182 @@
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
       <c r="O78" s="4"/>
-      <c r="P78" s="11"/>
+      <c r="P78" s="9"/>
     </row>
     <row r="79" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D79" s="5" t="s">
         <v>70</v>
       </c>
       <c r="E79" s="4"/>
-      <c r="F79" s="10"/>
+      <c r="F79" s="8"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
-      <c r="I79" s="19" t="s">
+      <c r="I79" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
-      <c r="M79" s="19"/>
-      <c r="N79" s="19" t="s">
+      <c r="M79" s="17"/>
+      <c r="N79" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O79" s="4"/>
-      <c r="P79" s="11"/>
+      <c r="P79" s="9"/>
     </row>
     <row r="80" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D80" s="6" t="s">
+      <c r="D80" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E80" s="7"/>
-      <c r="F80" s="10"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="8"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
-      <c r="I80" s="19" t="s">
+      <c r="I80" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
-      <c r="M80" s="19"/>
-      <c r="N80" s="19" t="s">
+      <c r="M80" s="17"/>
+      <c r="N80" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O80" s="4"/>
-      <c r="P80" s="11"/>
+      <c r="P80" s="9"/>
     </row>
     <row r="81" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D81" s="6" t="s">
+      <c r="D81" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E81" s="7"/>
-      <c r="F81" s="10"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="8"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
-      <c r="I81" s="19" t="s">
+      <c r="I81" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
-      <c r="M81" s="19"/>
-      <c r="N81" s="19" t="s">
+      <c r="M81" s="17"/>
+      <c r="N81" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O81" s="4"/>
-      <c r="P81" s="11"/>
+      <c r="P81" s="9"/>
     </row>
     <row r="82" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="10"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="8"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
-      <c r="I82" s="19" t="s">
+      <c r="I82" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
       <c r="L82" s="4"/>
-      <c r="M82" s="19"/>
-      <c r="N82" s="19" t="s">
+      <c r="M82" s="17"/>
+      <c r="N82" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O82" s="4"/>
-      <c r="P82" s="11"/>
+      <c r="P82" s="9"/>
     </row>
     <row r="83" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D83" s="6" t="s">
+      <c r="D83" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E83" s="7"/>
-      <c r="F83" s="10"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="8"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="19" t="s">
+      <c r="I83" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
       <c r="L83" s="4"/>
-      <c r="M83" s="19"/>
-      <c r="N83" s="19" t="s">
+      <c r="M83" s="17"/>
+      <c r="N83" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O83" s="4"/>
-      <c r="P83" s="11"/>
+      <c r="P83" s="9"/>
     </row>
     <row r="84" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E84" s="7"/>
-      <c r="F84" s="10"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="8"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="19" t="s">
+      <c r="I84" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
       <c r="L84" s="4"/>
-      <c r="M84" s="19"/>
-      <c r="N84" s="19" t="s">
+      <c r="M84" s="17"/>
+      <c r="N84" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O84" s="4"/>
-      <c r="P84" s="11"/>
+      <c r="P84" s="9"/>
     </row>
     <row r="85" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D85" s="6" t="s">
+      <c r="D85" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E85" s="7"/>
-      <c r="F85" s="10"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="8"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
-      <c r="I85" s="19" t="s">
+      <c r="I85" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
       <c r="L85" s="4"/>
-      <c r="M85" s="19"/>
-      <c r="N85" s="19" t="s">
+      <c r="M85" s="17"/>
+      <c r="N85" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O85" s="4"/>
-      <c r="P85" s="11"/>
+      <c r="P85" s="9"/>
     </row>
     <row r="86" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E86" s="7"/>
-      <c r="F86" s="10"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="8"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
-      <c r="I86" s="19" t="s">
+      <c r="I86" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
-      <c r="M86" s="19"/>
-      <c r="N86" s="19" t="s">
+      <c r="M86" s="17"/>
+      <c r="N86" s="17" t="s">
         <v>114</v>
       </c>
       <c r="O86" s="4"/>
-      <c r="P86" s="11"/>
+      <c r="P86" s="9"/>
     </row>
     <row r="87" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E87" s="4"/>
-      <c r="F87" s="10"/>
+      <c r="F87" s="8"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -3130,17 +4117,17 @@
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
       <c r="O87" s="4"/>
-      <c r="P87" s="11"/>
+      <c r="P87" s="9"/>
     </row>
     <row r="88" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D88" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E88" s="4"/>
-      <c r="F88" s="10"/>
+      <c r="F88" s="8"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
-      <c r="I88" s="19" t="s">
+      <c r="I88" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J88" s="4"/>
@@ -3149,17 +4136,17 @@
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
       <c r="O88" s="4"/>
-      <c r="P88" s="11"/>
+      <c r="P88" s="9"/>
     </row>
     <row r="89" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="10"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="8"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
-      <c r="I89" s="19" t="s">
+      <c r="I89" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J89" s="4"/>
@@ -3168,17 +4155,17 @@
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
-      <c r="P89" s="11"/>
+      <c r="P89" s="9"/>
     </row>
     <row r="90" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D90" s="6" t="s">
+      <c r="D90" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E90" s="7"/>
-      <c r="F90" s="10"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="8"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="19" t="s">
+      <c r="I90" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J90" s="4"/>
@@ -3187,17 +4174,17 @@
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
       <c r="O90" s="4"/>
-      <c r="P90" s="11"/>
+      <c r="P90" s="9"/>
     </row>
     <row r="91" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="E91" s="7"/>
-      <c r="F91" s="10"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="8"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="19" t="s">
+      <c r="I91" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J91" s="4"/>
@@ -3206,17 +4193,17 @@
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
       <c r="O91" s="4"/>
-      <c r="P91" s="11"/>
+      <c r="P91" s="9"/>
     </row>
     <row r="92" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D92" s="6" t="s">
+      <c r="D92" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="10"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="8"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="19" t="s">
+      <c r="I92" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J92" s="4"/>
@@ -3225,17 +4212,17 @@
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
       <c r="O92" s="4"/>
-      <c r="P92" s="11"/>
+      <c r="P92" s="9"/>
     </row>
     <row r="93" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D93" s="6" t="s">
+      <c r="D93" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E93" s="7"/>
-      <c r="F93" s="10"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="8"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
-      <c r="I93" s="19" t="s">
+      <c r="I93" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J93" s="4"/>
@@ -3244,17 +4231,17 @@
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
       <c r="O93" s="4"/>
-      <c r="P93" s="11"/>
+      <c r="P93" s="9"/>
     </row>
     <row r="94" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D94" s="6" t="s">
+      <c r="D94" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E94" s="7"/>
-      <c r="F94" s="10"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="8"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
-      <c r="I94" s="19" t="s">
+      <c r="I94" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J94" s="4"/>
@@ -3263,17 +4250,17 @@
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
       <c r="O94" s="4"/>
-      <c r="P94" s="11"/>
+      <c r="P94" s="9"/>
     </row>
     <row r="95" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D95" s="5" t="s">
         <v>86</v>
       </c>
       <c r="E95" s="4"/>
-      <c r="F95" s="10"/>
+      <c r="F95" s="8"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
-      <c r="I95" s="19" t="s">
+      <c r="I95" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J95" s="4"/>
@@ -3282,17 +4269,17 @@
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
-      <c r="P95" s="11"/>
+      <c r="P95" s="9"/>
     </row>
     <row r="96" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D96" s="6" t="s">
+      <c r="D96" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E96" s="7"/>
-      <c r="F96" s="10"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="8"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-      <c r="I96" s="19" t="s">
+      <c r="I96" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J96" s="4"/>
@@ -3301,17 +4288,17 @@
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
       <c r="O96" s="4"/>
-      <c r="P96" s="11"/>
+      <c r="P96" s="9"/>
     </row>
     <row r="97" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D97" s="6" t="s">
+      <c r="D97" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E97" s="7"/>
-      <c r="F97" s="10"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="8"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
-      <c r="I97" s="19" t="s">
+      <c r="I97" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J97" s="4"/>
@@ -3320,17 +4307,17 @@
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
       <c r="O97" s="4"/>
-      <c r="P97" s="11"/>
+      <c r="P97" s="9"/>
     </row>
     <row r="98" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D98" s="6" t="s">
+      <c r="D98" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E98" s="7"/>
-      <c r="F98" s="10"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="8"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
-      <c r="I98" s="19" t="s">
+      <c r="I98" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J98" s="4"/>
@@ -3339,17 +4326,17 @@
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
       <c r="O98" s="4"/>
-      <c r="P98" s="11"/>
+      <c r="P98" s="9"/>
     </row>
     <row r="99" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D99" s="6" t="s">
+      <c r="D99" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E99" s="7"/>
-      <c r="F99" s="10"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="8"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
-      <c r="I99" s="19" t="s">
+      <c r="I99" s="17" t="s">
         <v>114</v>
       </c>
       <c r="J99" s="4"/>
@@ -3358,14 +4345,14 @@
       <c r="M99" s="4"/>
       <c r="N99" s="4"/>
       <c r="O99" s="4"/>
-      <c r="P99" s="11"/>
+      <c r="P99" s="9"/>
     </row>
     <row r="100" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D100" s="8" t="s">
+      <c r="D100" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E100" s="4"/>
-      <c r="F100" s="10"/>
+      <c r="F100" s="8"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
@@ -3375,14 +4362,14 @@
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
       <c r="O100" s="4"/>
-      <c r="P100" s="11"/>
+      <c r="P100" s="9"/>
     </row>
     <row r="101" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D101" s="6" t="s">
+      <c r="D101" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="E101" s="7"/>
-      <c r="F101" s="10"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="8"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -3392,14 +4379,14 @@
       <c r="M101" s="4"/>
       <c r="N101" s="4"/>
       <c r="O101" s="4"/>
-      <c r="P101" s="11"/>
+      <c r="P101" s="9"/>
     </row>
     <row r="102" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D102" s="6" t="s">
+      <c r="D102" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="E102" s="7"/>
-      <c r="F102" s="10"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="8"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
@@ -3409,14 +4396,14 @@
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
-      <c r="P102" s="11"/>
+      <c r="P102" s="9"/>
     </row>
     <row r="103" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D103" s="6" t="s">
+      <c r="D103" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E103" s="7"/>
-      <c r="F103" s="10"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="8"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
@@ -3426,14 +4413,14 @@
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
       <c r="O103" s="4"/>
-      <c r="P103" s="11"/>
+      <c r="P103" s="9"/>
     </row>
     <row r="104" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D104" s="6" t="s">
+      <c r="D104" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E104" s="7"/>
-      <c r="F104" s="10"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="8"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -3443,14 +4430,14 @@
       <c r="M104" s="4"/>
       <c r="N104" s="4"/>
       <c r="O104" s="4"/>
-      <c r="P104" s="11"/>
+      <c r="P104" s="9"/>
     </row>
     <row r="105" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D105" s="6" t="s">
+      <c r="D105" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E105" s="7"/>
-      <c r="F105" s="10"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="8"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
@@ -3460,14 +4447,14 @@
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
       <c r="O105" s="4"/>
-      <c r="P105" s="11"/>
+      <c r="P105" s="9"/>
     </row>
     <row r="106" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D106" s="6" t="s">
+      <c r="D106" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E106" s="7"/>
-      <c r="F106" s="10"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="8"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
@@ -3477,14 +4464,14 @@
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
       <c r="O106" s="4"/>
-      <c r="P106" s="11"/>
+      <c r="P106" s="9"/>
     </row>
     <row r="107" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D107" s="6" t="s">
+      <c r="D107" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="E107" s="7"/>
-      <c r="F107" s="10"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="8"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
@@ -3494,14 +4481,14 @@
       <c r="M107" s="4"/>
       <c r="N107" s="4"/>
       <c r="O107" s="4"/>
-      <c r="P107" s="11"/>
+      <c r="P107" s="9"/>
     </row>
     <row r="108" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D108" s="6" t="s">
+      <c r="D108" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E108" s="7"/>
-      <c r="F108" s="10"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="8"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
@@ -3511,14 +4498,14 @@
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
       <c r="O108" s="4"/>
-      <c r="P108" s="11"/>
+      <c r="P108" s="9"/>
     </row>
     <row r="109" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D109" s="6" t="s">
+      <c r="D109" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="E109" s="7"/>
-      <c r="F109" s="10"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="8"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
@@ -3528,14 +4515,14 @@
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
       <c r="O109" s="4"/>
-      <c r="P109" s="11"/>
+      <c r="P109" s="9"/>
     </row>
     <row r="110" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D110" s="8" t="s">
+      <c r="D110" s="6" t="s">
         <v>101</v>
       </c>
       <c r="E110" s="4"/>
-      <c r="F110" s="10"/>
+      <c r="F110" s="8"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
@@ -3545,14 +4532,14 @@
       <c r="M110" s="4"/>
       <c r="N110" s="4"/>
       <c r="O110" s="4"/>
-      <c r="P110" s="11"/>
+      <c r="P110" s="9"/>
     </row>
     <row r="111" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D111" s="5" t="s">
         <v>102</v>
       </c>
       <c r="E111" s="4"/>
-      <c r="F111" s="10"/>
+      <c r="F111" s="8"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -3562,14 +4549,14 @@
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
       <c r="O111" s="4"/>
-      <c r="P111" s="11"/>
+      <c r="P111" s="9"/>
     </row>
     <row r="112" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D112" s="6" t="s">
+      <c r="D112" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E112" s="7"/>
-      <c r="F112" s="10"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="8"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -3579,14 +4566,14 @@
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
       <c r="O112" s="4"/>
-      <c r="P112" s="11"/>
+      <c r="P112" s="9"/>
     </row>
     <row r="113" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D113" s="6" t="s">
+      <c r="D113" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="E113" s="7"/>
-      <c r="F113" s="10"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="8"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
@@ -3596,14 +4583,14 @@
       <c r="M113" s="4"/>
       <c r="N113" s="4"/>
       <c r="O113" s="4"/>
-      <c r="P113" s="11"/>
+      <c r="P113" s="9"/>
     </row>
     <row r="114" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D114" s="6" t="s">
+      <c r="D114" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="E114" s="7"/>
-      <c r="F114" s="10"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="8"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
@@ -3613,14 +4600,14 @@
       <c r="M114" s="4"/>
       <c r="N114" s="4"/>
       <c r="O114" s="4"/>
-      <c r="P114" s="11"/>
+      <c r="P114" s="9"/>
     </row>
     <row r="115" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D115" s="8" t="s">
+      <c r="D115" s="6" t="s">
         <v>106</v>
       </c>
       <c r="E115" s="4"/>
-      <c r="F115" s="10"/>
+      <c r="F115" s="8"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -3630,14 +4617,14 @@
       <c r="M115" s="4"/>
       <c r="N115" s="4"/>
       <c r="O115" s="4"/>
-      <c r="P115" s="11"/>
+      <c r="P115" s="9"/>
     </row>
     <row r="116" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D116" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E116" s="4"/>
-      <c r="F116" s="10"/>
+      <c r="F116" s="8"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
@@ -3647,14 +4634,14 @@
       <c r="M116" s="4"/>
       <c r="N116" s="4"/>
       <c r="O116" s="4"/>
-      <c r="P116" s="11"/>
+      <c r="P116" s="9"/>
     </row>
     <row r="117" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D117" s="6" t="s">
+      <c r="D117" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="E117" s="7"/>
-      <c r="F117" s="10"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="8"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -3664,14 +4651,14 @@
       <c r="M117" s="4"/>
       <c r="N117" s="4"/>
       <c r="O117" s="4"/>
-      <c r="P117" s="11"/>
+      <c r="P117" s="9"/>
     </row>
     <row r="118" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D118" s="6" t="s">
+      <c r="D118" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="E118" s="7"/>
-      <c r="F118" s="10"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="8"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -3681,14 +4668,14 @@
       <c r="M118" s="4"/>
       <c r="N118" s="4"/>
       <c r="O118" s="4"/>
-      <c r="P118" s="11"/>
+      <c r="P118" s="9"/>
     </row>
     <row r="119" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D119" s="6" t="s">
+      <c r="D119" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="E119" s="7"/>
-      <c r="F119" s="10"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="8"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -3698,37 +4685,100 @@
       <c r="M119" s="4"/>
       <c r="N119" s="4"/>
       <c r="O119" s="4"/>
-      <c r="P119" s="11"/>
+      <c r="P119" s="9"/>
     </row>
     <row r="120" spans="4:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D120" s="6" t="s">
+      <c r="D120" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="E120" s="7"/>
-      <c r="F120" s="15"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="16"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
-      <c r="M120" s="16"/>
-      <c r="N120" s="16"/>
-      <c r="O120" s="16"/>
-      <c r="P120" s="17"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+      <c r="J120" s="14"/>
+      <c r="K120" s="14"/>
+      <c r="L120" s="14"/>
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+      <c r="O120" s="14"/>
+      <c r="P120" s="15"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="89">
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
     <mergeCell ref="D113:E113"/>
     <mergeCell ref="D99:E99"/>
     <mergeCell ref="D101:E101"/>
@@ -3736,78 +4786,16 @@
     <mergeCell ref="D103:E103"/>
     <mergeCell ref="D104:E104"/>
     <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3815,4 +4803,319 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEB4DE5C-847C-4BE7-87CC-F267FAE101AB}">
+  <dimension ref="C3:T6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C3" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D3" s="20" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_FV(C3,"52 week high",TRUE)</f>
+        <v>1159.44</v>
+      </c>
+      <c r="E3" s="20" cm="1">
+        <f t="array" aca="1" ref="E3" ca="1">_FV(C3,"52 week low",TRUE)</f>
+        <v>555.59</v>
+      </c>
+      <c r="F3" s="20" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">_FV(C3,"Change")</f>
+        <v>23.02</v>
+      </c>
+      <c r="G3" s="21" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">_FV(C3,"Change % (Extended hours)",TRUE)</f>
+        <v>-9.683999999999999E-4</v>
+      </c>
+      <c r="H3" s="21" cm="1">
+        <f t="array" aca="1" ref="H3" ca="1">_FV(C3,"Change (%)",TRUE)</f>
+        <v>2.0309000000000001E-2</v>
+      </c>
+      <c r="I3" s="20" cm="1">
+        <f t="array" aca="1" ref="I3" ca="1">_FV(C3,"Change (Extended hours)",TRUE)</f>
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="J3" t="str" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">_FV(C3,"Currency")</f>
+        <v>USD</v>
+      </c>
+      <c r="K3" t="str" cm="1">
+        <f t="array" aca="1" ref="K3" ca="1">_FV(C3,"Exchange")</f>
+        <v>Nasdaq Stock Market</v>
+      </c>
+      <c r="L3" s="20" cm="1">
+        <f t="array" aca="1" ref="L3" ca="1">_FV(C3,"High")</f>
+        <v>1159.44</v>
+      </c>
+      <c r="M3" s="20" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">_FV(C3,"Low")</f>
+        <v>1133.32</v>
+      </c>
+      <c r="N3" s="20" cm="1">
+        <f t="array" aca="1" ref="N3" ca="1">_FV(C3,"Open")</f>
+        <v>1136.6600000000001</v>
+      </c>
+      <c r="O3" s="20" cm="1">
+        <f t="array" aca="1" ref="O3" ca="1">_FV(C3,"Previous close",TRUE)</f>
+        <v>1133.47</v>
+      </c>
+      <c r="P3" s="20" cm="1">
+        <f t="array" aca="1" ref="P3" ca="1">_FV(C3,"Price")</f>
+        <v>1156.49</v>
+      </c>
+      <c r="Q3" s="20" cm="1">
+        <f t="array" aca="1" ref="Q3" ca="1">_FV(C3,"Price (Extended hours)",TRUE)</f>
+        <v>1155.3699999999999</v>
+      </c>
+      <c r="R3" t="str" cm="1">
+        <f t="array" aca="1" ref="R3" ca="1">_FV(C3,"Ticker symbol",TRUE)</f>
+        <v>NFLX</v>
+      </c>
+      <c r="S3" s="22" cm="1">
+        <f t="array" aca="1" ref="S3" ca="1">_FV(C3,"Volume")</f>
+        <v>3769325</v>
+      </c>
+      <c r="T3" s="22" cm="1">
+        <f t="array" aca="1" ref="T3" ca="1">_FV(C3,"Volume average",TRUE)</f>
+        <v>5542343</v>
+      </c>
+    </row>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C4" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4" s="20" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_FV(C4,"52 week high",TRUE)</f>
+        <v>468.35</v>
+      </c>
+      <c r="E4" s="20" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">_FV(C4,"52 week low",TRUE)</f>
+        <v>344.79</v>
+      </c>
+      <c r="F4" s="20" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">_FV(C4,"Change")</f>
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="G4" s="21" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">_FV(C4,"Change % (Extended hours)",TRUE)</f>
+        <v>-5.2839999999999994E-4</v>
+      </c>
+      <c r="H4" s="21" cm="1">
+        <f t="array" aca="1" ref="H4" ca="1">_FV(C4,"Change (%)",TRUE)</f>
+        <v>2.3224999999999999E-2</v>
+      </c>
+      <c r="I4" s="20" cm="1">
+        <f t="array" aca="1" ref="I4" ca="1">_FV(C4,"Change (Extended hours)",TRUE)</f>
+        <v>-0.23</v>
+      </c>
+      <c r="J4" t="str" cm="1">
+        <f t="array" aca="1" ref="J4" ca="1">_FV(C4,"Currency")</f>
+        <v>USD</v>
+      </c>
+      <c r="K4" t="str" cm="1">
+        <f t="array" aca="1" ref="K4" ca="1">_FV(C4,"Exchange")</f>
+        <v>Nasdaq Stock Market</v>
+      </c>
+      <c r="L4" s="20" cm="1">
+        <f t="array" aca="1" ref="L4" ca="1">_FV(C4,"High")</f>
+        <v>439.44</v>
+      </c>
+      <c r="M4" s="20" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">_FV(C4,"Low")</f>
+        <v>429.98500000000001</v>
+      </c>
+      <c r="N4" s="20" cm="1">
+        <f t="array" aca="1" ref="N4" ca="1">_FV(C4,"Open")</f>
+        <v>431.74</v>
+      </c>
+      <c r="O4" s="20" cm="1">
+        <f t="array" aca="1" ref="O4" ca="1">_FV(C4,"Previous close",TRUE)</f>
+        <v>425.4</v>
+      </c>
+      <c r="P4" s="20" cm="1">
+        <f t="array" aca="1" ref="P4" ca="1">_FV(C4,"Price")</f>
+        <v>435.28</v>
+      </c>
+      <c r="Q4" s="20" cm="1">
+        <f t="array" aca="1" ref="Q4" ca="1">_FV(C4,"Price (Extended hours)",TRUE)</f>
+        <v>435.05</v>
+      </c>
+      <c r="R4" t="str" cm="1">
+        <f t="array" aca="1" ref="R4" ca="1">_FV(C4,"Ticker symbol",TRUE)</f>
+        <v>MSFT</v>
+      </c>
+      <c r="S4" s="22" cm="1">
+        <f t="array" aca="1" ref="S4" ca="1">_FV(C4,"Volume")</f>
+        <v>30747812</v>
+      </c>
+      <c r="T4" s="22" cm="1">
+        <f t="array" aca="1" ref="T4" ca="1">_FV(C4,"Volume average",TRUE)</f>
+        <v>27706619</v>
+      </c>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C5" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5" s="20" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_FV(C5,"52 week high",TRUE)</f>
+        <v>242.52</v>
+      </c>
+      <c r="E5" s="20" cm="1">
+        <f t="array" aca="1" ref="E5" ca="1">_FV(C5,"52 week low",TRUE)</f>
+        <v>151.61000000000001</v>
+      </c>
+      <c r="F5" s="20" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">_FV(C5,"Change")</f>
+        <v>-0.22</v>
+      </c>
+      <c r="G5" s="21" cm="1">
+        <f t="array" aca="1" ref="G5" ca="1">_FV(C5,"Change % (Extended hours)",TRUE)</f>
+        <v>-1.5789999999999999E-4</v>
+      </c>
+      <c r="H5" s="21" cm="1">
+        <f t="array" aca="1" ref="H5" ca="1">_FV(C5,"Change (%)",TRUE)</f>
+        <v>-1.157E-3</v>
+      </c>
+      <c r="I5" s="20" cm="1">
+        <f t="array" aca="1" ref="I5" ca="1">_FV(C5,"Change (Extended hours)",TRUE)</f>
+        <v>-0.03</v>
+      </c>
+      <c r="J5" t="str" cm="1">
+        <f t="array" aca="1" ref="J5" ca="1">_FV(C5,"Currency")</f>
+        <v>USD</v>
+      </c>
+      <c r="K5" t="str" cm="1">
+        <f t="array" aca="1" ref="K5" ca="1">_FV(C5,"Exchange")</f>
+        <v>Nasdaq Stock Market</v>
+      </c>
+      <c r="L5" s="20" cm="1">
+        <f t="array" aca="1" ref="L5" ca="1">_FV(C5,"High")</f>
+        <v>192.88</v>
+      </c>
+      <c r="M5" s="20" cm="1">
+        <f t="array" aca="1" ref="M5" ca="1">_FV(C5,"Low")</f>
+        <v>186.4</v>
+      </c>
+      <c r="N5" s="20" cm="1">
+        <f t="array" aca="1" ref="N5" ca="1">_FV(C5,"Open")</f>
+        <v>191.435</v>
+      </c>
+      <c r="O5" s="20" cm="1">
+        <f t="array" aca="1" ref="O5" ca="1">_FV(C5,"Previous close",TRUE)</f>
+        <v>190.2</v>
+      </c>
+      <c r="P5" s="20" cm="1">
+        <f t="array" aca="1" ref="P5" ca="1">_FV(C5,"Price")</f>
+        <v>189.98</v>
+      </c>
+      <c r="Q5" s="20" cm="1">
+        <f t="array" aca="1" ref="Q5" ca="1">_FV(C5,"Price (Extended hours)",TRUE)</f>
+        <v>189.95</v>
+      </c>
+      <c r="R5" t="str" cm="1">
+        <f t="array" aca="1" ref="R5" ca="1">_FV(C5,"Ticker symbol",TRUE)</f>
+        <v>AMZN</v>
+      </c>
+      <c r="S5" s="22" cm="1">
+        <f t="array" aca="1" ref="S5" ca="1">_FV(C5,"Volume")</f>
+        <v>77843282</v>
+      </c>
+      <c r="T5" s="22" cm="1">
+        <f t="array" aca="1" ref="T5" ca="1">_FV(C5,"Volume average",TRUE)</f>
+        <v>61230915</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C6" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D6" s="20" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_FV(C6,"52 week high",TRUE)</f>
+        <v>488.53989999999999</v>
+      </c>
+      <c r="E6" s="20" cm="1">
+        <f t="array" aca="1" ref="E6" ca="1">_FV(C6,"52 week low",TRUE)</f>
+        <v>167.41</v>
+      </c>
+      <c r="F6" s="20" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">_FV(C6,"Change")</f>
+        <v>6.69</v>
+      </c>
+      <c r="G6" s="21" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">_FV(C6,"Change % (Extended hours)",TRUE)</f>
+        <v>1.7060000000000001E-3</v>
+      </c>
+      <c r="H6" s="21" cm="1">
+        <f t="array" aca="1" ref="H6" ca="1">_FV(C6,"Change (%)",TRUE)</f>
+        <v>2.3848999999999999E-2</v>
+      </c>
+      <c r="I6" s="20" cm="1">
+        <f t="array" aca="1" ref="I6" ca="1">_FV(C6,"Change (Extended hours)",TRUE)</f>
+        <v>0.49</v>
+      </c>
+      <c r="J6" t="str" cm="1">
+        <f t="array" aca="1" ref="J6" ca="1">_FV(C6,"Currency")</f>
+        <v>USD</v>
+      </c>
+      <c r="K6" t="str" cm="1">
+        <f t="array" aca="1" ref="K6" ca="1">_FV(C6,"Exchange")</f>
+        <v>Nasdaq Stock Market</v>
+      </c>
+      <c r="L6" s="20" cm="1">
+        <f t="array" aca="1" ref="L6" ca="1">_FV(C6,"High")</f>
+        <v>294.77999999999997</v>
+      </c>
+      <c r="M6" s="20" cm="1">
+        <f t="array" aca="1" ref="M6" ca="1">_FV(C6,"Low")</f>
+        <v>279.81</v>
+      </c>
+      <c r="N6" s="20" cm="1">
+        <f t="array" aca="1" ref="N6" ca="1">_FV(C6,"Open")</f>
+        <v>284.89999999999998</v>
+      </c>
+      <c r="O6" s="20" cm="1">
+        <f t="array" aca="1" ref="O6" ca="1">_FV(C6,"Previous close",TRUE)</f>
+        <v>280.52</v>
+      </c>
+      <c r="P6" s="20" cm="1">
+        <f t="array" aca="1" ref="P6" ca="1">_FV(C6,"Price")</f>
+        <v>287.20999999999998</v>
+      </c>
+      <c r="Q6" s="20" cm="1">
+        <f t="array" aca="1" ref="Q6" ca="1">_FV(C6,"Price (Extended hours)",TRUE)</f>
+        <v>287.7</v>
+      </c>
+      <c r="R6" t="str" cm="1">
+        <f t="array" aca="1" ref="R6" ca="1">_FV(C6,"Ticker symbol",TRUE)</f>
+        <v>TSLA</v>
+      </c>
+      <c r="S6" s="22" cm="1">
+        <f t="array" aca="1" ref="S6" ca="1">_FV(C6,"Volume")</f>
+        <v>114214271</v>
+      </c>
+      <c r="T6" s="22" cm="1">
+        <f t="array" aca="1" ref="T6" ca="1">_FV(C6,"Volume average",TRUE)</f>
+        <v>139121393</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>